<commit_message>
Added the coulomb potential
</commit_message>
<xml_diff>
--- a/input_files/Ca40_RMF.xlsx
+++ b/input_files/Ca40_RMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Projects/Light-Front Mean Field Theory/Runge-Kutta Method/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AF91DB-04B3-AF4F-9132-51A9D069C47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01E59CA-0672-7C43-8D43-34F6409F2AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="9340" windowWidth="28800" windowHeight="15640" activeTab="1" xr2:uid="{178560A9-F361-274A-AB9D-3DA0C106A5E5}"/>
+    <workbookView xWindow="6960" yWindow="4100" windowWidth="28800" windowHeight="15640" activeTab="3" xr2:uid="{178560A9-F361-274A-AB9D-3DA0C106A5E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
     <t>COULOMB STRENGTH [MEV]</t>
   </si>
   <si>
-    <t>COULOMBCOUPLING</t>
+    <t>COULOMB COUPLING</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603E9AEF-BC4E-8547-A3F8-1FD6EEDF1358}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,7 +660,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -752,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -772,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -792,7 +792,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -812,7 +812,7 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF253CE-956B-B040-8027-78DFB140BDDF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,10 +867,10 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -889,10 +889,10 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -911,10 +911,10 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -931,10 +931,10 @@
         <v>22</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -971,10 +971,10 @@
         <v>24</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the case where we get solution to Dirac equation in 0 iterations. Now we can solve O16, Ca40, and Pb208.
</commit_message>
<xml_diff>
--- a/input_files/Ca40_RMF.xlsx
+++ b/input_files/Ca40_RMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Projects/Light-Front Mean Field Theory/Runge-Kutta Method/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23213D91-4759-E042-84B0-DE177F9E3569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED70BE5E-24E4-3648-B04C-6F4BF206EFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="4100" windowWidth="28800" windowHeight="15640" activeTab="1" xr2:uid="{178560A9-F361-274A-AB9D-3DA0C106A5E5}"/>
+    <workbookView xWindow="6960" yWindow="4100" windowWidth="28800" windowHeight="15640" activeTab="3" xr2:uid="{178560A9-F361-274A-AB9D-3DA0C106A5E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="G2">
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -570,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603E9AEF-BC4E-8547-A3F8-1FD6EEDF1358}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -660,7 +660,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,14 +698,14 @@
         <v>-1</v>
       </c>
       <c r="C2">
-        <f>850</f>
-        <v>850</v>
+        <f>877</f>
+        <v>877</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0.5</v>
@@ -727,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>0.5</v>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>0.5</v>
@@ -769,7 +769,7 @@
         <v>22</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>0.5</v>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF253CE-956B-B040-8027-78DFB140BDDF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,14 +860,14 @@
         <v>-1</v>
       </c>
       <c r="C2">
-        <f>850</f>
-        <v>850</v>
+        <f>877</f>
+        <v>877</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>-0.5</v>
@@ -889,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>-0.5</v>
@@ -911,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>-0.5</v>
@@ -931,7 +931,7 @@
         <v>22</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>-0.5</v>

</xml_diff>